<commit_message>
Group tests now insert correctly.  Fixed error in VolAddress
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
+++ b/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
@@ -29,7 +29,7 @@
     <t>Query</t>
   </si>
   <si>
-    <t>[VolTeer].[Vol].[GroupAddr]</t>
+    <t>[VolTeer].[Vol].[tblGroupAddr]</t>
   </si>
 </sst>
 </file>
@@ -39,7 +39,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -61,12 +61,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,7 +110,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,7 +134,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -174,7 +168,7 @@
       </c>
       <c r="D2" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '100','6')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '100','6')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,7 +184,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '101','2')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '101','2')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,7 +200,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '102','3')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '102','3')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,11 +212,11 @@
         <v>103</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '103','25')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '103','9')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,7 +232,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '104','5')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '104','5')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,7 +248,7 @@
       </c>
       <c r="D7" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '105','6')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '105','6')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +264,7 @@
       </c>
       <c r="D8" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '106','7')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '106','7')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,11 +276,11 @@
         <v>107</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '107','18')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '107','8')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,7 +296,7 @@
       </c>
       <c r="D10" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '108','2')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '108','2')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,7 +312,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[GroupAddr] ([GroupID],[AddrID]) VALUES ( '110','4')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '110','4')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Group UTs.  Added missing/untracked xlsx files to repo
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
+++ b/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Table</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>AddrID</t>
+  </si>
+  <si>
+    <t>PrimaryAddrID</t>
+  </si>
+  <si>
+    <t>ActiveFlg</t>
   </si>
   <si>
     <t>Query</t>
@@ -131,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -155,10 +161,16 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>100</v>
@@ -166,14 +178,20 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '100','6')</v>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '100','6','1','1')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2+1</f>
@@ -182,14 +200,20 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '101','2')</v>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "','" &amp; E3 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '101','2','0','1')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+1</f>
@@ -198,14 +222,20 @@
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '102','3')</v>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "','" &amp; E4 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '102','3','1','1')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B4+1</f>
@@ -214,14 +244,20 @@
       <c r="C5" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '103','9')</v>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '103','9','1','1')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B5+1</f>
@@ -230,14 +266,20 @@
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '104','5')</v>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '104','5','1','1')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6+1</f>
@@ -246,14 +288,20 @@
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '105','6')</v>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "','" &amp; E7 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '105','6','0','1')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7+1</f>
@@ -262,14 +310,20 @@
       <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '106','7')</v>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "','" &amp; E8 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '106','7','1','0')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B8+1</f>
@@ -278,14 +332,20 @@
       <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '107','8')</v>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "','" &amp; E9 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '107','8','1','1')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B9+1</f>
@@ -294,14 +354,20 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '108','2')</v>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "','" &amp; E10 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '108','2','0','1')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+2</f>
@@ -310,9 +376,15 @@
       <c r="C11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '110','4')</v>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "','" &amp; E11 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '110','4','1','1')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PrimaryAddrID to GroupAddr
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
+++ b/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>Table</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>AddrID</t>
+  </si>
+  <si>
+    <t>PrimaryAddrID</t>
   </si>
   <si>
     <t>Query</t>
@@ -131,10 +134,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -155,10 +158,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>100</v>
@@ -166,14 +172,17 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '100','6')</v>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '100','6','1')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2+1</f>
@@ -182,14 +191,17 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '101','2')</v>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '101','2','1')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+1</f>
@@ -198,14 +210,17 @@
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '102','3')</v>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '102','3','1')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B4+1</f>
@@ -214,14 +229,17 @@
       <c r="C5" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '103','9')</v>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '103','9','1')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B5+1</f>
@@ -230,14 +248,17 @@
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '104','5')</v>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '104','5','1')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6+1</f>
@@ -246,14 +267,17 @@
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '105','6')</v>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '105','6','1')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7+1</f>
@@ -262,14 +286,17 @@
       <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '106','7')</v>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '106','7','1')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B8+1</f>
@@ -278,14 +305,17 @@
       <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '107','8')</v>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '107','8','1')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B9+1</f>
@@ -294,14 +324,17 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '108','2')</v>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '108','2','1')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+2</f>
@@ -310,9 +343,12 @@
       <c r="C11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID]) VALUES ( '110','4')</v>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '110','4','1')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of fixes to the UTs
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
+++ b/UT.Vol.BLL/HelperFiles/GroupAddr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Table</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>PrimaryAddrID</t>
+  </si>
+  <si>
+    <t>ActiveFlg</t>
   </si>
   <si>
     <t>Query</t>
@@ -134,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -161,10 +164,13 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>100</v>
@@ -175,14 +181,17 @@
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '100','6','1')</v>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '100','6','1','1')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2+1</f>
@@ -194,14 +203,17 @@
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '101','2','1')</v>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "','" &amp; E3 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '101','2','1','1')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+1</f>
@@ -213,14 +225,17 @@
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '102','3','1')</v>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "','" &amp; E4 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '102','3','1','1')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B4+1</f>
@@ -232,14 +247,17 @@
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '103','9','1')</v>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '103','9','1','1')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B5+1</f>
@@ -251,14 +269,17 @@
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '104','5','1')</v>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '104','5','1','1')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6+1</f>
@@ -270,14 +291,17 @@
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '105','6','1')</v>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "','" &amp; E7 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '105','6','1','1')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7+1</f>
@@ -289,14 +313,17 @@
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '106','7','1')</v>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "','" &amp; E8 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '106','7','1','1')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B8+1</f>
@@ -308,14 +335,17 @@
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '107','8','1')</v>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "','" &amp; E9 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '107','8','1','1')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B9+1</f>
@@ -327,14 +357,17 @@
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '108','2','1')</v>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "','" &amp; E10 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '108','2','1','1')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+2</f>
@@ -346,9 +379,12 @@
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="str">
-        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "')"</f>
-        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID]) VALUES ( '110','4','1')</v>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "','" &amp; E11 &amp; "')"</f>
+        <v>INSERT INTO [VolTeer].[Vol].[tblGroupAddr] ([GroupID],[AddrID],[PrimaryAddrID],[ActiveFlg]) VALUES ( '110','4','1','1')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>